<commit_message>
backend finish con fronted
</commit_message>
<xml_diff>
--- a/Backend/app/data/data.xlsx
+++ b/Backend/app/data/data.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="usuarios" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,30 +15,20 @@
     <sheet name="ordenes_pedido" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -51,42 +42,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -99,20 +60,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -481,35 +436,35 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>nombre</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>contraseña</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>rol</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>fecha_registro</t>
         </is>
@@ -541,7 +496,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-12-15 14:39:37</t>
+          <t>2024-12-16 07:48:02</t>
         </is>
       </c>
     </row>
@@ -556,20 +511,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col width="16.28515625" customWidth="1" min="2" max="2"/>
-    <col width="21.5703125" customWidth="1" min="3" max="3"/>
-    <col width="18.28515625" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="6"/>
-    <col width="19.7109375" customWidth="1" min="7" max="7"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -579,7 +527,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>nombre_producto</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -600,11 +548,6 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>fecha_agregado</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>fecha_actualizado</t>
         </is>
       </c>
     </row>
@@ -630,7 +573,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -656,7 +599,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -682,7 +625,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -708,7 +651,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -734,7 +677,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -758,32 +701,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>nombre</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nombre_materia_prima</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>cantidad_disponible</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>precio_por_unidad</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>producto_id</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>fecha_agregado</t>
         </is>
@@ -806,6 +749,11 @@
       </c>
       <c r="E2" t="n">
         <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -826,6 +774,11 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -837,13 +790,18 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D4" t="n">
         <v>0.5</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -856,13 +814,18 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>0.2</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -875,13 +838,18 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D6" t="n">
         <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>3</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -894,13 +862,18 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D7" t="n">
         <v>0.05</v>
       </c>
       <c r="E7" t="n">
         <v>3</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -921,6 +894,11 @@
       <c r="E8" t="n">
         <v>4</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -940,6 +918,11 @@
       <c r="E9" t="n">
         <v>4</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -959,6 +942,11 @@
       <c r="E10" t="n">
         <v>5</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -977,6 +965,11 @@
       </c>
       <c r="E11" t="n">
         <v>5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024-12-16 07:47:47</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -993,17 +986,10 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col width="20.5703125" customWidth="1" min="2" max="2"/>
-    <col width="18.5703125" customWidth="1" min="3" max="3"/>
-    <col width="21.140625" customWidth="1" min="4" max="4"/>
-    <col width="16.85546875" customWidth="1" min="5" max="5"/>
-    <col width="24" customWidth="1" min="6" max="6"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1057,7 +1043,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1067,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -1105,7 +1091,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1115,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1139,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1163,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-12-15 14:37:03</t>
+          <t>2024-12-16 07:47:47</t>
         </is>
       </c>
     </row>
@@ -1198,12 +1184,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col width="16.5703125" customWidth="1" min="2" max="2"/>
-    <col width="14.5703125" customWidth="1" min="3" max="3"/>
-    <col width="24.42578125" customWidth="1" min="4" max="4"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1310,7 +1291,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,52 +1300,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>usuario_id</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>producto_id</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>cantidad</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>total_costos_directos</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>total_costos_indirectos</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>total_costos</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>precio_unitario</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>fecha_entrega</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>fecha_creacion</t>
         </is>
@@ -1378,22 +1359,22 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>167</v>
+        <v>44.5</v>
       </c>
       <c r="F2" t="n">
         <v>700</v>
       </c>
       <c r="G2" t="n">
-        <v>867</v>
+        <v>744.5</v>
       </c>
       <c r="H2" t="n">
-        <v>86.7</v>
+        <v>74.45</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -1402,7 +1383,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2024-12-15 14:43:37</t>
+          <t>2024-12-16 07:48:12</t>
         </is>
       </c>
     </row>
@@ -1414,22 +1395,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
         <v>2</v>
       </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
       <c r="E3" t="n">
-        <v>51.5</v>
+        <v>125.4</v>
       </c>
       <c r="F3" t="n">
         <v>700</v>
       </c>
       <c r="G3" t="n">
-        <v>751.5</v>
+        <v>825.4</v>
       </c>
       <c r="H3" t="n">
-        <v>75.15000000000001</v>
+        <v>412.7</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -1438,7 +1419,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2024-12-15 17:06:32</t>
+          <t>2024-12-16 07:48:51</t>
         </is>
       </c>
     </row>
@@ -1453,19 +1434,19 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>127.45</v>
+        <v>121.3</v>
       </c>
       <c r="F4" t="n">
         <v>700</v>
       </c>
       <c r="G4" t="n">
-        <v>827.45</v>
+        <v>821.3</v>
       </c>
       <c r="H4" t="n">
-        <v>827.45</v>
+        <v>410.65</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -1474,259 +1455,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2024-12-15 17:57:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>123.35</v>
-      </c>
-      <c r="F5" t="n">
-        <v>700</v>
-      </c>
-      <c r="G5" t="n">
-        <v>823.35</v>
-      </c>
-      <c r="H5" t="n">
-        <v>411.675</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:57:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>113.1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>700</v>
-      </c>
-      <c r="G6" t="n">
-        <v>813.1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>162.62</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:58:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" t="n">
-        <v>100.8</v>
-      </c>
-      <c r="F7" t="n">
-        <v>700</v>
-      </c>
-      <c r="G7" t="n">
-        <v>800.8</v>
-      </c>
-      <c r="H7" t="n">
-        <v>133.4666666666667</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:58:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" t="n">
-        <v>80.3</v>
-      </c>
-      <c r="F8" t="n">
-        <v>700</v>
-      </c>
-      <c r="G8" t="n">
-        <v>780.3</v>
-      </c>
-      <c r="H8" t="n">
-        <v>78.03</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:58:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>78.25</v>
-      </c>
-      <c r="F9" t="n">
-        <v>700</v>
-      </c>
-      <c r="G9" t="n">
-        <v>778.25</v>
-      </c>
-      <c r="H9" t="n">
-        <v>778.25</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:58:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" t="n">
-        <v>5</v>
-      </c>
-      <c r="E10" t="n">
-        <v>68.25</v>
-      </c>
-      <c r="F10" t="n">
-        <v>700</v>
-      </c>
-      <c r="G10" t="n">
-        <v>768.25</v>
-      </c>
-      <c r="H10" t="n">
-        <v>153.65</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:58:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>66.2</v>
-      </c>
-      <c r="F11" t="n">
-        <v>700</v>
-      </c>
-      <c r="G11" t="n">
-        <v>766.2</v>
-      </c>
-      <c r="H11" t="n">
-        <v>766.2</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>2024-12-15 17:58:55</t>
+          <t>2024-12-16 08:01:21</t>
         </is>
       </c>
     </row>

</xml_diff>